<commit_message>
Add new columns name
</commit_message>
<xml_diff>
--- a/combined_output.xlsx
+++ b/combined_output.xlsx
@@ -440,12 +440,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Grand Prix</t>
+          <t>Grand_prix</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Race_date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -460,7 +460,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Race_time</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">

</xml_diff>